<commit_message>
various fixes and improvements
git-svn-id: https://source.sunlightlabs.com/subsidyscope@506 8399c101-ab5c-441d-b403-44365f039031
</commit_message>
<xml_diff>
--- a/etl/h41/misc/fedh41_v3.xlsx
+++ b/etl/h41/misc/fedh41_v3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36460" yWindow="-420" windowWidth="21600" windowHeight="14300" tabRatio="500" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="-35680" yWindow="-280" windowWidth="21600" windowHeight="14340" tabRatio="500" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -219,15 +219,15 @@
   </si>
   <si>
     <t>date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>non-bailout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Treasury securities, Fed. Agency debt securities, Repurchase agreements &amp; some other loans</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -240,13 +240,27 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="5">
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
     <font>
       <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="14"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="11"/>
       <name val="Verdana"/>
     </font>
   </fonts>
@@ -270,9 +284,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -23546,7 +23565,7 @@
                   <c:v>25785.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31.0</c:v>
+                  <c:v>26980.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>27131.0</c:v>
@@ -24415,6 +24434,9 @@
                 <c:pt idx="3">
                   <c:v>27464.0</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>27037.0</c:v>
+                </c:pt>
                 <c:pt idx="5">
                   <c:v>26946.0</c:v>
                 </c:pt>
@@ -28602,6 +28624,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>388791.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>465853.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -29405,7 +29430,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr published="0"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -35027,8 +35052,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -39250,7 +39274,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -42784,7 +42809,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -42799,8 +42825,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Y114"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -43208,145 +43234,152 @@
         <v>542467</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:25" s="3" customFormat="1">
+      <c r="A6" s="5">
         <v>38380</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>1989877</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>475200</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>26668</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>17143</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>64990</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <v>34</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="6">
         <v>1</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
         <v>44428</v>
       </c>
-      <c r="L6" s="1">
+      <c r="K6" s="6"/>
+      <c r="L6" s="5">
         <f t="shared" si="0"/>
         <v>38380</v>
       </c>
-      <c r="M6">
-        <v>31</v>
-      </c>
-      <c r="N6">
+      <c r="M6" s="4">
+        <v>26980</v>
+      </c>
+      <c r="N6" s="4">
         <v>19692</v>
       </c>
-      <c r="P6">
+      <c r="O6" s="4">
+        <v>27037</v>
+      </c>
+      <c r="P6" s="6">
         <v>26668</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="6">
         <v>32054</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="6">
         <v>14593</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="6">
         <v>38336</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="6">
         <v>6824</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="6">
         <v>316201</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="6">
         <v>415859</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="6">
         <v>44428</v>
       </c>
-      <c r="Y6">
+      <c r="X6" s="4">
+        <v>465853</v>
+      </c>
+      <c r="Y6" s="6">
         <f t="shared" si="1"/>
         <v>557368</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:25" s="3" customFormat="1">
+      <c r="A7" s="2">
         <v>38373</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>2049246</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>475381</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>24158</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>37143</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>61618</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>74</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>1</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
         <v>520184</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="2">
         <f t="shared" si="0"/>
         <v>38373</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="3">
         <v>27131</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="3">
         <v>19802</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="3">
         <v>26946</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="3">
         <v>24158</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="3">
         <v>32679</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="3">
         <v>15482</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="3">
         <v>38445</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="3">
         <v>5784</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="3">
         <v>349940</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="3">
         <v>416031</v>
       </c>
-      <c r="W7">
+      <c r="W7" s="3">
         <v>520184</v>
       </c>
-      <c r="Y7">
+      <c r="Y7" s="3">
         <f t="shared" si="1"/>
         <v>574217</v>
       </c>
@@ -47896,7 +47929,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>